<commit_message>
Fix Formula in Sample manifest
</commit_message>
<xml_diff>
--- a/docs/Volundr Sample Manifest Template.xlsx
+++ b/docs/Volundr Sample Manifest Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Volundr/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="613" documentId="8_{AA74DB3A-68E0-4BAE-8893-84B0905BE785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF6FC875-BCE2-4E84-9DA0-2FC4C8F51CAE}"/>
+  <xr:revisionPtr revIDLastSave="617" documentId="8_{AA74DB3A-68E0-4BAE-8893-84B0905BE785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE1D1576-161D-4201-91C7-9BD0BBC7AC3C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{EBA5DD3A-97B6-4850-B85A-CEA820199B58}"/>
   </bookViews>
@@ -1259,9 +1259,6 @@
     <t>Reverse Phasing</t>
   </si>
   <si>
-    <t># Synthetic Lethal Sample Manifest v0.7.0</t>
-  </si>
-  <si>
     <t>Forward Phasing</t>
   </si>
   <si>
@@ -1278,6 +1275,9 @@
   </si>
   <si>
     <t>CTGACAAT</t>
+  </si>
+  <si>
+    <t># Synthetic Lethal Sample Manifest v0.7.1</t>
   </si>
 </sst>
 </file>
@@ -2430,7 +2430,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2451,7 +2451,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="B1" s="24"/>
       <c r="E1" s="22"/>
@@ -2498,7 +2498,10 @@
         <v>304</v>
       </c>
       <c r="H4" s="46"/>
-      <c r="I4" s="28"/>
+      <c r="I4" s="28">
+        <f>I3-SUMIF(J9:J104,"&lt;&gt;#DIV/0!")</f>
+        <v>0</v>
+      </c>
       <c r="J4" s="8"/>
       <c r="K4" s="21"/>
     </row>
@@ -2558,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>405</v>
@@ -2588,8 +2591,14 @@
       <c r="F9" s="42"/>
       <c r="G9" s="16"/>
       <c r="H9" s="18"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
+      <c r="I9" s="17" t="e">
+        <f t="shared" ref="I9:I74" si="0">((G9*0.000000001)/(H9*660))*1000000000000000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="17" t="e">
+        <f t="shared" ref="J9:J73" si="1">(I$2/I9)*(I$3/COUNT(I$9:I$104))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="K9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -2601,8 +2610,14 @@
       <c r="F10" s="42"/>
       <c r="G10" s="16"/>
       <c r="H10" s="18"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="I10" s="17" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -2615,11 +2630,11 @@
       <c r="G11" s="16"/>
       <c r="H11" s="18"/>
       <c r="I11" s="17" t="e">
-        <f t="shared" ref="I11:I74" si="0">((G11*0.000000001)/(H11*660))*1000000000000000</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J11" s="17" t="e">
-        <f t="shared" ref="J10:J73" si="1">(I$2/I11)*(I$3/COUNT(I$9:I$104))</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K11" s="23"/>
@@ -4657,7 +4672,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>405</v>
@@ -4680,7 +4695,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>10</v>
@@ -4692,10 +4707,10 @@
         <v>6</v>
       </c>
       <c r="E9" s="39" t="s">
+        <v>410</v>
+      </c>
+      <c r="F9" s="39" t="s">
         <v>411</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>412</v>
       </c>
       <c r="G9" s="16">
         <v>1</v>
@@ -4715,7 +4730,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>205</v>
@@ -4742,7 +4757,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>10</v>

</xml_diff>